<commit_message>
Adicion de pestaña de modelo de process_yield
</commit_message>
<xml_diff>
--- a/knowledge_module/modal_specs/modal_specs.xlsx
+++ b/knowledge_module/modal_specs/modal_specs.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="71">
   <si>
     <t>D04_total_residue</t>
   </si>
@@ -198,6 +198,48 @@
   </si>
   <si>
     <t>Regenerator drop pressure (in H2O)</t>
+  </si>
+  <si>
+    <t>yield</t>
+  </si>
+  <si>
+    <t>D03_cuero</t>
+  </si>
+  <si>
+    <t>D09_T_liquor</t>
+  </si>
+  <si>
+    <t>D10_T_out_gelatin</t>
+  </si>
+  <si>
+    <t>D10_T_out_water</t>
+  </si>
+  <si>
+    <t>D12_P_atom_regn</t>
+  </si>
+  <si>
+    <t>D12_P_filt</t>
+  </si>
+  <si>
+    <t>Leather as raw material</t>
+  </si>
+  <si>
+    <t>Liqueur temperature paraflash (ºC)</t>
+  </si>
+  <si>
+    <t>Sterilizer gelatin outflow temperature (ºC)</t>
+  </si>
+  <si>
+    <t>Sterilizer water outflow temperature (ºC)</t>
+  </si>
+  <si>
+    <t>Regenerator atomization pressure (psi)</t>
+  </si>
+  <si>
+    <t>Filter drop pressure (in H2O)</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -537,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,6 +1393,262 @@
         <v>38</v>
       </c>
     </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H26" t="s">
+        <v>35</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="1">
+        <v>50.277053140096598</v>
+      </c>
+      <c r="G27" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" t="s">
+        <v>35</v>
+      </c>
+      <c r="I27">
+        <v>50.277053140096598</v>
+      </c>
+      <c r="J27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="1">
+        <v>20.8319082125603</v>
+      </c>
+      <c r="G28" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28">
+        <v>20.8319082125603</v>
+      </c>
+      <c r="J28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="1">
+        <v>4</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="1">
+        <v>48.176158204643897</v>
+      </c>
+      <c r="G29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29">
+        <v>48.176158204643897</v>
+      </c>
+      <c r="J29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="1">
+        <v>5</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="1">
+        <v>40.110690315408696</v>
+      </c>
+      <c r="G30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30">
+        <v>40.110690315408696</v>
+      </c>
+      <c r="J30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="1">
+        <v>6</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0.19253048079134999</v>
+      </c>
+      <c r="G31" t="s">
+        <v>32</v>
+      </c>
+      <c r="H31" t="s">
+        <v>35</v>
+      </c>
+      <c r="I31">
+        <v>0.19253048079134999</v>
+      </c>
+      <c r="J31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="1">
+        <v>7</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0.29206314699792901</v>
+      </c>
+      <c r="G32" t="s">
+        <v>32</v>
+      </c>
+      <c r="H32" t="s">
+        <v>35</v>
+      </c>
+      <c r="I32">
+        <v>0.29206314699792901</v>
+      </c>
+      <c r="J32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="1">
+        <v>8</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0.87258482861743702</v>
+      </c>
+      <c r="G33" t="s">
+        <v>32</v>
+      </c>
+      <c r="H33" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33">
+        <v>0.87258482861743702</v>
+      </c>
+      <c r="J33" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="119" orientation="portrait" r:id="rId1"/>

</xml_diff>